<commit_message>
fix example for dev workd
</commit_message>
<xml_diff>
--- a/test_example.xlsx
+++ b/test_example.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Redbock\Desktop\bmrn-test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD1CAF04-1243-4A4E-A660-44016C2C77D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="555" yWindow="3465" windowWidth="21600" windowHeight="11325" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Instruction" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Data entry sheet" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Example" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Instruction" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Entry" sheetId="2" r:id="rId2"/>
+    <sheet name="Example" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,212 +29,209 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="66">
   <si>
-    <t xml:space="preserve">In cell B1, please record the label for your endpoint or biomarker with unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the label that will be displayed on the y-axis of the output graphs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In cell D1, please record LLOQ if there are BLQ in your data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This should be a number only, no units.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grey cells are fixed text that cannot be changed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This describes the type of model used in the study (i.e. the genotype, genetic background or disease model used).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment group name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This describes the treatment, if any, that was administered to the subjects during the study. It will be included as text on the output graph.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the identifier for each subject (e.g. mouse) included in the study.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Techical Replicate ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If there are replicate measures for a subject, enter the replicate IDs here. This field can be left blank if there are no techinical replicates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose with units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the dosing information. It will be included as text on the output graphs. For subjects that are not dosed, leave blank.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the baseline measurement of your endpoint or biomarker (numbers only, do not include units). This field can be left blank if there is not baseline for the study.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time1, Time2….</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replace the text in these boxes with the time points for your study (including units). Input the endpoint or biomarker values for each subject in the rows below.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Example" sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review this sheet to see an example of what the data input looks like.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment Group Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubjectID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose with unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time1 (free text)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time2 (free text)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time3 (free text)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time4 (free text)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time5 (free text)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wild type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle</t>
+    <t>In cell B1, please record the label for your endpoint or biomarker with unit</t>
+  </si>
+  <si>
+    <t>This is the label that will be displayed on the y-axis of the output graphs.</t>
+  </si>
+  <si>
+    <t>In cell D1, please record LLOQ if there are BLQ in your data</t>
+  </si>
+  <si>
+    <t>This should be a number only, no units.</t>
+  </si>
+  <si>
+    <t>Grey cells are fixed text that cannot be changed.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>This describes the type of model used in the study (i.e. the genotype, genetic background or disease model used).</t>
+  </si>
+  <si>
+    <t>Treatment group name</t>
+  </si>
+  <si>
+    <t>This describes the treatment, if any, that was administered to the subjects during the study. It will be included as text on the output graph.</t>
+  </si>
+  <si>
+    <t>Subject ID</t>
+  </si>
+  <si>
+    <t>This is the identifier for each subject (e.g. mouse) included in the study.</t>
+  </si>
+  <si>
+    <t>Techical Replicate ID</t>
+  </si>
+  <si>
+    <t>If there are replicate measures for a subject, enter the replicate IDs here. This field can be left blank if there are no techinical replicates.</t>
+  </si>
+  <si>
+    <t>Dose with units</t>
+  </si>
+  <si>
+    <t>This is the dosing information. It will be included as text on the output graphs. For subjects that are not dosed, leave blank.</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>This is the baseline measurement of your endpoint or biomarker (numbers only, do not include units). This field can be left blank if there is not baseline for the study.</t>
+  </si>
+  <si>
+    <t>Time1, Time2….</t>
+  </si>
+  <si>
+    <t>Replace the text in these boxes with the time points for your study (including units). Input the endpoint or biomarker values for each subject in the rows below.</t>
+  </si>
+  <si>
+    <t>"Example" sheet</t>
+  </si>
+  <si>
+    <t>Review this sheet to see an example of what the data input looks like.</t>
+  </si>
+  <si>
+    <t>Treatment Group Name</t>
+  </si>
+  <si>
+    <t>SubjectID</t>
+  </si>
+  <si>
+    <t>Dose with unit</t>
+  </si>
+  <si>
+    <t>Time1 (free text)</t>
+  </si>
+  <si>
+    <t>Time2 (free text)</t>
+  </si>
+  <si>
+    <t>Time3 (free text)</t>
+  </si>
+  <si>
+    <t>Time4 (free text)</t>
+  </si>
+  <si>
+    <t>Time5 (free text)</t>
+  </si>
+  <si>
+    <t>Wild type</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
   </si>
   <si>
     <t xml:space="preserve">Disease </t>
   </si>
   <si>
-    <t xml:space="preserve">Negative Control</t>
+    <t>Negative Control</t>
   </si>
   <si>
     <t xml:space="preserve">Postive Control </t>
   </si>
   <si>
-    <t xml:space="preserve">Trt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">creatine kinase (ng/ml)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Replicate ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMN000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 mg/kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 mg/kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 mg/kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G3</t>
+    <t>Trt</t>
+  </si>
+  <si>
+    <t>creatine kinase (ng/ml)</t>
+  </si>
+  <si>
+    <t>Technical Replicate ID</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>4 weeks</t>
+  </si>
+  <si>
+    <t>6 weeks</t>
+  </si>
+  <si>
+    <t>8 weeks</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>BMN000</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>1 mg/kg</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>3 mg/kg</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>10 mg/kg</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -238,22 +240,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -261,7 +248,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -316,7 +303,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -324,113 +311,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -489,29 +431,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="60.14"/>
+    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -527,13 +777,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -541,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -549,7 +799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -557,7 +807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -565,7 +815,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -573,7 +823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -581,7 +831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -589,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -598,35 +848,27 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="6" width="9.14"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="6" customWidth="1"/>
+    <col min="3" max="11" width="9.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -635,7 +877,7 @@
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -670,7 +912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -679,7 +921,7 @@
       </c>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -688,7 +930,7 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>31</v>
       </c>
@@ -697,7 +939,7 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -706,7 +948,7 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -714,7 +956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
@@ -722,7 +964,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
@@ -730,7 +972,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
@@ -739,39 +981,31 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="A3:K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="6" width="9.14"/>
+    <col min="1" max="1" width="12.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="6" customWidth="1"/>
+    <col min="5" max="6" width="10.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="6" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="84" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -781,18 +1015,18 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="n">
+      <c r="D1" s="13">
         <v>20</v>
       </c>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="15"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" s="2" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -827,7 +1061,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -837,27 +1071,27 @@
       <c r="C4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="6">
         <v>20</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="6">
         <v>21</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="6">
         <v>22</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="6">
         <v>21</v>
       </c>
-      <c r="J4" s="6" t="n">
+      <c r="J4" s="6">
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -867,27 +1101,27 @@
       <c r="C5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="6">
         <v>2</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="6">
         <v>21</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="6">
         <v>24</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="6">
         <v>20</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="6">
         <v>20</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -897,27 +1131,27 @@
       <c r="C6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="6">
         <v>21</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="6">
         <v>24</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="6">
         <v>20</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="6">
         <v>20</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -927,27 +1161,27 @@
       <c r="C7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="6">
         <v>20</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="6">
         <v>24</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="6">
         <v>21</v>
       </c>
-      <c r="I7" s="6" t="n">
+      <c r="I7" s="6">
         <v>20</v>
       </c>
-      <c r="J7" s="6" t="n">
+      <c r="J7" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -957,27 +1191,27 @@
       <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="6">
         <v>20</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="6">
         <v>21</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="6">
         <v>20</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="6">
         <v>21</v>
       </c>
-      <c r="J8" s="6" t="n">
+      <c r="J8" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -987,27 +1221,27 @@
       <c r="C9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="6">
         <v>20</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="6">
         <v>21</v>
       </c>
-      <c r="H9" s="6" t="n">
+      <c r="H9" s="6">
         <v>20</v>
       </c>
-      <c r="I9" s="6" t="n">
+      <c r="I9" s="6">
         <v>21</v>
       </c>
-      <c r="J9" s="6" t="n">
+      <c r="J9" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
@@ -1017,27 +1251,27 @@
       <c r="C10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="6">
         <v>1</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="6">
         <v>50</v>
       </c>
-      <c r="G10" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H10" s="6" t="n">
+      <c r="G10" s="6">
+        <v>49</v>
+      </c>
+      <c r="H10" s="6">
         <v>52</v>
       </c>
-      <c r="I10" s="6" t="n">
+      <c r="I10" s="6">
         <v>60</v>
       </c>
-      <c r="J10" s="6" t="n">
+      <c r="J10" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
@@ -1047,27 +1281,27 @@
       <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="6">
         <v>2</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="6">
         <v>50</v>
       </c>
-      <c r="G11" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H11" s="6" t="n">
+      <c r="G11" s="6">
+        <v>49</v>
+      </c>
+      <c r="H11" s="6">
         <v>52</v>
       </c>
-      <c r="I11" s="6" t="n">
+      <c r="I11" s="6">
         <v>60</v>
       </c>
-      <c r="J11" s="6" t="n">
+      <c r="J11" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -1077,27 +1311,27 @@
       <c r="C12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="6" t="n">
+      <c r="F12" s="6">
         <v>58</v>
       </c>
-      <c r="G12" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H12" s="6" t="n">
+      <c r="G12" s="6">
+        <v>49</v>
+      </c>
+      <c r="H12" s="6">
         <v>52</v>
       </c>
-      <c r="I12" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="J12" s="6" t="n">
+      <c r="I12" s="6">
+        <v>49</v>
+      </c>
+      <c r="J12" s="6">
         <v>52</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
@@ -1107,27 +1341,27 @@
       <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="6">
         <v>2</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="6">
         <v>58</v>
       </c>
-      <c r="G13" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H13" s="6" t="n">
+      <c r="G13" s="6">
+        <v>49</v>
+      </c>
+      <c r="H13" s="6">
         <v>52</v>
       </c>
-      <c r="I13" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="J13" s="6" t="n">
+      <c r="I13" s="6">
+        <v>49</v>
+      </c>
+      <c r="J13" s="6">
         <v>52</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -1137,27 +1371,27 @@
       <c r="C14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="6">
         <v>1</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="6" t="n">
+      <c r="F14" s="6">
         <v>52</v>
       </c>
-      <c r="G14" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H14" s="6" t="n">
+      <c r="G14" s="6">
+        <v>49</v>
+      </c>
+      <c r="H14" s="6">
         <v>52</v>
       </c>
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="6">
         <v>58</v>
       </c>
-      <c r="J14" s="6" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
@@ -1167,27 +1401,27 @@
       <c r="C15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="6">
         <v>2</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="6">
         <v>47</v>
       </c>
-      <c r="G15" s="6" t="n">
+      <c r="G15" s="6">
         <v>56</v>
       </c>
-      <c r="H15" s="6" t="n">
+      <c r="H15" s="6">
         <v>53</v>
       </c>
-      <c r="I15" s="6" t="n">
+      <c r="I15" s="6">
         <v>58</v>
       </c>
-      <c r="J15" s="6" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
@@ -1197,27 +1431,27 @@
       <c r="C16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="H16" s="6" t="n">
+      <c r="F16" s="6">
+        <v>30</v>
+      </c>
+      <c r="G16" s="6">
+        <v>30</v>
+      </c>
+      <c r="H16" s="6">
         <v>27</v>
       </c>
-      <c r="I16" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J16" s="6" t="n">
+      <c r="I16" s="6">
+        <v>30</v>
+      </c>
+      <c r="J16" s="6">
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -1227,27 +1461,27 @@
       <c r="C17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="D17" s="6">
         <v>2</v>
       </c>
       <c r="E17" s="12"/>
-      <c r="F17" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G17" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="H17" s="6" t="n">
+      <c r="F17" s="6">
+        <v>30</v>
+      </c>
+      <c r="G17" s="6">
+        <v>31</v>
+      </c>
+      <c r="H17" s="6">
         <v>27</v>
       </c>
-      <c r="I17" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J17" s="6" t="n">
+      <c r="I17" s="6">
+        <v>30</v>
+      </c>
+      <c r="J17" s="6">
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -1257,27 +1491,27 @@
       <c r="C18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="12"/>
-      <c r="F18" s="6" t="n">
+      <c r="F18" s="6">
         <v>32</v>
       </c>
-      <c r="G18" s="6" t="n">
+      <c r="G18" s="6">
         <v>24</v>
       </c>
-      <c r="H18" s="6" t="n">
+      <c r="H18" s="6">
         <v>25</v>
       </c>
-      <c r="I18" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="J18" s="6" t="n">
+      <c r="I18" s="6">
+        <v>31</v>
+      </c>
+      <c r="J18" s="6">
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
@@ -1287,27 +1521,27 @@
       <c r="C19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="6" t="n">
+      <c r="D19" s="6">
         <v>2</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G19" s="6" t="n">
+      <c r="F19" s="6">
+        <v>30</v>
+      </c>
+      <c r="G19" s="6">
         <v>35</v>
       </c>
-      <c r="H19" s="6" t="n">
+      <c r="H19" s="6">
         <v>25</v>
       </c>
-      <c r="I19" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="J19" s="6" t="n">
+      <c r="I19" s="6">
+        <v>31</v>
+      </c>
+      <c r="J19" s="6">
         <v>35</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -1317,27 +1551,27 @@
       <c r="C20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="6" t="n">
+      <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="12"/>
-      <c r="F20" s="6" t="n">
+      <c r="F20" s="6">
         <v>38</v>
       </c>
-      <c r="G20" s="6" t="n">
+      <c r="G20" s="6">
         <v>36</v>
       </c>
-      <c r="H20" s="6" t="n">
+      <c r="H20" s="6">
         <v>28</v>
       </c>
-      <c r="I20" s="6" t="n">
+      <c r="I20" s="6">
         <v>34</v>
       </c>
-      <c r="J20" s="6" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
@@ -1347,27 +1581,27 @@
       <c r="C21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="6" t="n">
+      <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="12"/>
-      <c r="F21" s="6" t="n">
+      <c r="F21" s="6">
         <v>38</v>
       </c>
-      <c r="G21" s="6" t="n">
+      <c r="G21" s="6">
         <v>36</v>
       </c>
-      <c r="H21" s="6" t="n">
+      <c r="H21" s="6">
         <v>28</v>
       </c>
-      <c r="I21" s="6" t="n">
+      <c r="I21" s="6">
         <v>34</v>
       </c>
-      <c r="J21" s="6" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
@@ -1377,27 +1611,27 @@
       <c r="C22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="6" t="n">
+      <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="12"/>
-      <c r="F22" s="6" t="n">
+      <c r="F22" s="6">
         <v>50</v>
       </c>
-      <c r="G22" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H22" s="6" t="n">
+      <c r="G22" s="6">
+        <v>49</v>
+      </c>
+      <c r="H22" s="6">
         <v>52</v>
       </c>
-      <c r="I22" s="6" t="n">
+      <c r="I22" s="6">
         <v>60</v>
       </c>
-      <c r="J22" s="6" t="n">
+      <c r="J22" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>31</v>
       </c>
@@ -1407,27 +1641,27 @@
       <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D23" s="6">
         <v>2</v>
       </c>
       <c r="E23" s="12"/>
-      <c r="F23" s="6" t="n">
+      <c r="F23" s="6">
         <v>50</v>
       </c>
-      <c r="G23" s="6" t="n">
+      <c r="G23" s="6">
         <v>50</v>
       </c>
-      <c r="H23" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="I23" s="6" t="n">
+      <c r="H23" s="6">
+        <v>49</v>
+      </c>
+      <c r="I23" s="6">
         <v>55</v>
       </c>
-      <c r="J23" s="6" t="n">
+      <c r="J23" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
@@ -1437,27 +1671,27 @@
       <c r="C24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="6" t="n">
+      <c r="D24" s="6">
         <v>1</v>
       </c>
       <c r="E24" s="12"/>
-      <c r="F24" s="6" t="n">
+      <c r="F24" s="6">
         <v>58</v>
       </c>
-      <c r="G24" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H24" s="6" t="n">
+      <c r="G24" s="6">
+        <v>49</v>
+      </c>
+      <c r="H24" s="6">
         <v>52</v>
       </c>
-      <c r="I24" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="J24" s="6" t="n">
+      <c r="I24" s="6">
+        <v>49</v>
+      </c>
+      <c r="J24" s="6">
         <v>52</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -1467,27 +1701,27 @@
       <c r="C25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="6" t="n">
+      <c r="D25" s="6">
         <v>2</v>
       </c>
       <c r="E25" s="12"/>
-      <c r="F25" s="6" t="n">
+      <c r="F25" s="6">
         <v>58</v>
       </c>
-      <c r="G25" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H25" s="6" t="n">
+      <c r="G25" s="6">
+        <v>49</v>
+      </c>
+      <c r="H25" s="6">
         <v>52</v>
       </c>
-      <c r="I25" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="J25" s="6" t="n">
+      <c r="I25" s="6">
+        <v>49</v>
+      </c>
+      <c r="J25" s="6">
         <v>52</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -1497,27 +1731,27 @@
       <c r="C26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="6" t="n">
+      <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" s="12"/>
-      <c r="F26" s="6" t="n">
+      <c r="F26" s="6">
         <v>47</v>
       </c>
-      <c r="G26" s="6" t="n">
+      <c r="G26" s="6">
         <v>56</v>
       </c>
-      <c r="H26" s="6" t="n">
+      <c r="H26" s="6">
         <v>53</v>
       </c>
-      <c r="I26" s="6" t="n">
+      <c r="I26" s="6">
         <v>58</v>
       </c>
-      <c r="J26" s="6" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>31</v>
       </c>
@@ -1527,27 +1761,27 @@
       <c r="C27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D27" s="6">
         <v>2</v>
       </c>
       <c r="E27" s="12"/>
-      <c r="F27" s="6" t="n">
+      <c r="F27" s="6">
         <v>47</v>
       </c>
-      <c r="G27" s="6" t="n">
+      <c r="G27" s="6">
         <v>56</v>
       </c>
-      <c r="H27" s="6" t="n">
+      <c r="H27" s="6">
         <v>53</v>
       </c>
-      <c r="I27" s="6" t="n">
+      <c r="I27" s="6">
         <v>58</v>
       </c>
-      <c r="J27" s="6" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1557,29 +1791,29 @@
       <c r="C28" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="6" t="n">
+      <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="6" t="n">
+      <c r="F28" s="6">
         <v>50</v>
       </c>
-      <c r="G28" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H28" s="6" t="n">
+      <c r="G28" s="6">
+        <v>49</v>
+      </c>
+      <c r="H28" s="6">
         <v>52</v>
       </c>
-      <c r="I28" s="6" t="n">
+      <c r="I28" s="6">
         <v>60</v>
       </c>
-      <c r="J28" s="6" t="n">
+      <c r="J28" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
@@ -1589,29 +1823,29 @@
       <c r="C29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="6" t="n">
+      <c r="D29" s="6">
         <v>2</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="6" t="n">
+      <c r="F29" s="6">
         <v>50</v>
       </c>
-      <c r="G29" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H29" s="6" t="n">
+      <c r="G29" s="6">
+        <v>49</v>
+      </c>
+      <c r="H29" s="6">
         <v>52</v>
       </c>
-      <c r="I29" s="6" t="n">
+      <c r="I29" s="6">
         <v>60</v>
       </c>
-      <c r="J29" s="6" t="n">
+      <c r="J29" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>31</v>
       </c>
@@ -1621,29 +1855,29 @@
       <c r="C30" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="6" t="n">
+      <c r="D30" s="6">
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="6" t="n">
+      <c r="F30" s="6">
         <v>58</v>
       </c>
-      <c r="G30" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H30" s="6" t="n">
+      <c r="G30" s="6">
+        <v>49</v>
+      </c>
+      <c r="H30" s="6">
         <v>52</v>
       </c>
-      <c r="I30" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="J30" s="6" t="n">
+      <c r="I30" s="6">
+        <v>49</v>
+      </c>
+      <c r="J30" s="6">
         <v>52</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -1653,29 +1887,29 @@
       <c r="C31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D31" s="6">
         <v>2</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="6" t="n">
+      <c r="F31" s="6">
         <v>58</v>
       </c>
-      <c r="G31" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="H31" s="6" t="n">
+      <c r="G31" s="6">
+        <v>49</v>
+      </c>
+      <c r="H31" s="6">
         <v>52</v>
       </c>
-      <c r="I31" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="J31" s="6" t="n">
+      <c r="I31" s="6">
+        <v>49</v>
+      </c>
+      <c r="J31" s="6">
         <v>52</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
@@ -1685,29 +1919,29 @@
       <c r="C32" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="6" t="n">
+      <c r="D32" s="6">
         <v>1</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="6" t="n">
+      <c r="F32" s="6">
         <v>47</v>
       </c>
-      <c r="G32" s="6" t="n">
+      <c r="G32" s="6">
         <v>56</v>
       </c>
-      <c r="H32" s="6" t="n">
+      <c r="H32" s="6">
         <v>53</v>
       </c>
-      <c r="I32" s="6" t="n">
+      <c r="I32" s="6">
         <v>58</v>
       </c>
-      <c r="J32" s="6" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -1717,29 +1951,29 @@
       <c r="C33" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="6" t="n">
+      <c r="D33" s="6">
         <v>2</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="6" t="n">
+      <c r="F33" s="6">
         <v>47</v>
       </c>
-      <c r="G33" s="6" t="n">
+      <c r="G33" s="6">
         <v>56</v>
       </c>
-      <c r="H33" s="6" t="n">
+      <c r="H33" s="6">
         <v>53</v>
       </c>
-      <c r="I33" s="6" t="n">
+      <c r="I33" s="6">
         <v>58</v>
       </c>
-      <c r="J33" s="6" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>31</v>
       </c>
@@ -1749,29 +1983,29 @@
       <c r="C34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="6" t="n">
+      <c r="D34" s="6">
         <v>1</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="6" t="n">
+      <c r="F34" s="6">
         <v>40</v>
       </c>
-      <c r="G34" s="6" t="n">
+      <c r="G34" s="6">
         <v>43</v>
       </c>
-      <c r="H34" s="6" t="n">
+      <c r="H34" s="6">
         <v>40</v>
       </c>
-      <c r="I34" s="6" t="n">
+      <c r="I34" s="6">
         <v>43</v>
       </c>
-      <c r="J34" s="6" t="n">
+      <c r="J34" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>31</v>
       </c>
@@ -1781,29 +2015,29 @@
       <c r="C35" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="6" t="n">
+      <c r="D35" s="6">
         <v>2</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="6" t="n">
+      <c r="F35" s="6">
         <v>40</v>
       </c>
-      <c r="G35" s="6" t="n">
+      <c r="G35" s="6">
         <v>43</v>
       </c>
-      <c r="H35" s="6" t="n">
+      <c r="H35" s="6">
         <v>40</v>
       </c>
-      <c r="I35" s="6" t="n">
+      <c r="I35" s="6">
         <v>43</v>
       </c>
-      <c r="J35" s="6" t="n">
+      <c r="J35" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>31</v>
       </c>
@@ -1813,29 +2047,29 @@
       <c r="C36" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D36" s="6">
         <v>1</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="6" t="n">
+      <c r="F36" s="6">
         <v>42</v>
       </c>
-      <c r="G36" s="6" t="n">
+      <c r="G36" s="6">
         <v>43</v>
       </c>
-      <c r="H36" s="6" t="n">
+      <c r="H36" s="6">
         <v>42</v>
       </c>
-      <c r="I36" s="6" t="n">
+      <c r="I36" s="6">
         <v>43</v>
       </c>
-      <c r="J36" s="6" t="n">
+      <c r="J36" s="6">
         <v>42</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -1845,29 +2079,29 @@
       <c r="C37" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="6" t="n">
+      <c r="D37" s="6">
         <v>2</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="6" t="n">
+      <c r="F37" s="6">
         <v>42</v>
       </c>
-      <c r="G37" s="6" t="n">
+      <c r="G37" s="6">
         <v>43</v>
       </c>
-      <c r="H37" s="6" t="n">
+      <c r="H37" s="6">
         <v>42</v>
       </c>
-      <c r="I37" s="6" t="n">
+      <c r="I37" s="6">
         <v>43</v>
       </c>
-      <c r="J37" s="6" t="n">
+      <c r="J37" s="6">
         <v>42</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>31</v>
       </c>
@@ -1877,29 +2111,29 @@
       <c r="C38" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="6" t="n">
+      <c r="D38" s="6">
         <v>1</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F38" s="6" t="n">
+      <c r="F38" s="6">
         <v>40</v>
       </c>
-      <c r="G38" s="6" t="n">
+      <c r="G38" s="6">
         <v>41</v>
       </c>
-      <c r="H38" s="6" t="n">
+      <c r="H38" s="6">
         <v>40</v>
       </c>
-      <c r="I38" s="6" t="n">
+      <c r="I38" s="6">
         <v>41</v>
       </c>
-      <c r="J38" s="6" t="n">
+      <c r="J38" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>31</v>
       </c>
@@ -1909,29 +2143,29 @@
       <c r="C39" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="6" t="n">
+      <c r="D39" s="6">
         <v>2</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="6" t="n">
+      <c r="F39" s="6">
         <v>40</v>
       </c>
-      <c r="G39" s="6" t="n">
+      <c r="G39" s="6">
         <v>41</v>
       </c>
-      <c r="H39" s="6" t="n">
+      <c r="H39" s="6">
         <v>40</v>
       </c>
-      <c r="I39" s="6" t="n">
+      <c r="I39" s="6">
         <v>41</v>
       </c>
-      <c r="J39" s="6" t="n">
+      <c r="J39" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>31</v>
       </c>
@@ -1941,29 +2175,29 @@
       <c r="C40" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="6" t="n">
+      <c r="D40" s="6">
         <v>1</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G40" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="H40" s="6" t="n">
+      <c r="F40" s="6">
+        <v>30</v>
+      </c>
+      <c r="G40" s="6">
+        <v>31</v>
+      </c>
+      <c r="H40" s="6">
         <v>27</v>
       </c>
-      <c r="I40" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J40" s="6" t="n">
+      <c r="I40" s="6">
+        <v>30</v>
+      </c>
+      <c r="J40" s="6">
         <v>29</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>31</v>
       </c>
@@ -1973,29 +2207,29 @@
       <c r="C41" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="6" t="n">
+      <c r="D41" s="6">
         <v>2</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G41" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="H41" s="6" t="n">
+      <c r="F41" s="6">
+        <v>30</v>
+      </c>
+      <c r="G41" s="6">
+        <v>31</v>
+      </c>
+      <c r="H41" s="6">
         <v>27</v>
       </c>
-      <c r="I41" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J41" s="6" t="n">
+      <c r="I41" s="6">
+        <v>30</v>
+      </c>
+      <c r="J41" s="6">
         <v>29</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>31</v>
       </c>
@@ -2005,29 +2239,29 @@
       <c r="C42" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="6" t="n">
+      <c r="D42" s="6">
         <v>1</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G42" s="6" t="n">
+      <c r="F42" s="6">
+        <v>30</v>
+      </c>
+      <c r="G42" s="6">
         <v>35</v>
       </c>
-      <c r="H42" s="6" t="n">
+      <c r="H42" s="6">
         <v>25</v>
       </c>
-      <c r="I42" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="J42" s="6" t="n">
+      <c r="I42" s="6">
+        <v>31</v>
+      </c>
+      <c r="J42" s="6">
         <v>35</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>31</v>
       </c>
@@ -2037,29 +2271,29 @@
       <c r="C43" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="6" t="n">
+      <c r="D43" s="6">
         <v>2</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="G43" s="6" t="n">
+      <c r="F43" s="6">
+        <v>30</v>
+      </c>
+      <c r="G43" s="6">
         <v>35</v>
       </c>
-      <c r="H43" s="6" t="n">
+      <c r="H43" s="6">
         <v>25</v>
       </c>
-      <c r="I43" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="J43" s="6" t="n">
+      <c r="I43" s="6">
+        <v>31</v>
+      </c>
+      <c r="J43" s="6">
         <v>35</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>31</v>
       </c>
@@ -2069,29 +2303,29 @@
       <c r="C44" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="6" t="n">
+      <c r="D44" s="6">
         <v>1</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="6" t="n">
+      <c r="F44" s="6">
         <v>38</v>
       </c>
-      <c r="G44" s="6" t="n">
+      <c r="G44" s="6">
         <v>36</v>
       </c>
-      <c r="H44" s="6" t="n">
+      <c r="H44" s="6">
         <v>28</v>
       </c>
-      <c r="I44" s="6" t="n">
+      <c r="I44" s="6">
         <v>34</v>
       </c>
-      <c r="J44" s="6" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J44" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>31</v>
       </c>
@@ -2101,38 +2335,33 @@
       <c r="C45" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="6" t="n">
+      <c r="D45" s="6">
         <v>2</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F45" s="6" t="n">
+      <c r="F45" s="6">
         <v>38</v>
       </c>
-      <c r="G45" s="6" t="n">
+      <c r="G45" s="6">
         <v>36</v>
       </c>
-      <c r="H45" s="6" t="n">
+      <c r="H45" s="6">
         <v>28</v>
       </c>
-      <c r="I45" s="6" t="n">
+      <c r="I45" s="6">
         <v>34</v>
       </c>
-      <c r="J45" s="6" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J45" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>